<commit_message>
git commit -m "casedetail moved to separate brnch"
</commit_message>
<xml_diff>
--- a/InputFiles/TC25_Canine_Filter_Breed-Greyhnd.xlsx
+++ b/InputFiles/TC25_Canine_Filter_Breed-Greyhnd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65BC7C2E-7252-4F7D-939C-521E8A827C9C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765925A7-D97B-4885-B2FF-B8C12C519850}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>WebExcel</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WHERE demo.breed IN['Greyhound']  OPTIONAL MATCH (f:file)-[*]-&gt;(c), (samp:sample)-[*]-&gt;(c) WITH DISTINCT c AS c, p, s, demo, diag, f, samp RETURN count(DISTINCT(f)) as number_of_files , count(DISTINCT(samp)) as number_of_sample , count(DISTINCT(c.case_id)) as number_of_cases , count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
+  </si>
+  <si>
+    <t>caseDetailQuery</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)-[*]-&gt;(c:case) WITH DISTINCT(f) AS f, c MATCH (f)--&gt;(parent) WHERE c.case_id IN ['caseid'] RETURN f.file_name AS `File Name` ,f.file_type AS `File Type`,head(labels(parent)) AS `Association`, f.file_description AS `Description`,f.file_format AS Format,((f.file_size)/1024) AS Size</t>
   </si>
 </sst>
 </file>
@@ -424,20 +430,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="75.81640625" customWidth="1"/>
-    <col min="3" max="3" width="70.26953125" customWidth="1"/>
-    <col min="4" max="4" width="28.54296875" customWidth="1"/>
+    <col min="1" max="3" width="75.81640625" customWidth="1"/>
+    <col min="4" max="4" width="70.26953125" customWidth="1"/>
+    <col min="5" max="5" width="28.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -445,23 +451,29 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="174" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>